<commit_message>
Updated spreadsheet with Ranking Point aggregates.
</commit_message>
<xml_diff>
--- a/tba/tba_push_into_excel_template.xlsx
+++ b/tba/tba_push_into_excel_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnhurrell/Development/fairport-robotics/ScoutingPASSSync/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnhurrell/Development/fairport-robotics/ScoutingPASSSync/tba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3758B5E-7893-B44A-BE8F-C579A02B20C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B73AF5-8F69-4B48-9202-6F46F7ECC466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MatchScoutingData" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MatchScoutingData!$A$1:$AE$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'PB Scouter Summary'!$A$1:$B$101</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'PB Team Summary'!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Team Scores'!$A$3:$AO$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Team Summary'!$A$3:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Team Scores'!$A$3:$AR$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Team Summary'!$A$3:$U$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Teams!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
   <si>
     <t>Key</t>
   </si>
@@ -300,6 +300,21 @@
   <si>
     <t>Match Count</t>
   </si>
+  <si>
+    <t>Ranking Points</t>
+  </si>
+  <si>
+    <t>Coral</t>
+  </si>
+  <si>
+    <t>Barge</t>
+  </si>
+  <si>
+    <t>Ranking Points Scored</t>
+  </si>
+  <si>
+    <t>Ranking Points Percentile</t>
+  </si>
 </sst>
 </file>
 
@@ -347,7 +362,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,8 +405,20 @@
         <bgColor rgb="FF229954"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor rgb="FFD68910"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -532,11 +559,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90"/>
@@ -613,6 +649,16 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -673,6 +719,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1013,9 +1060,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE999"/>
+  <dimension ref="A1:AE998"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -34018,39 +34065,6 @@
       <c r="AD998" s="3"/>
       <c r="AE998" s="3"/>
     </row>
-    <row r="999" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A999" s="2"/>
-      <c r="B999" s="3"/>
-      <c r="C999" s="3"/>
-      <c r="D999" s="3"/>
-      <c r="E999" s="3"/>
-      <c r="F999" s="3"/>
-      <c r="G999" s="3"/>
-      <c r="H999" s="3"/>
-      <c r="I999" s="3"/>
-      <c r="J999" s="3"/>
-      <c r="K999" s="3"/>
-      <c r="L999" s="3"/>
-      <c r="M999" s="3"/>
-      <c r="N999" s="3"/>
-      <c r="O999" s="3"/>
-      <c r="P999" s="3"/>
-      <c r="Q999" s="3"/>
-      <c r="R999" s="3"/>
-      <c r="S999" s="3"/>
-      <c r="T999" s="3"/>
-      <c r="U999" s="3"/>
-      <c r="V999" s="3"/>
-      <c r="W999" s="3"/>
-      <c r="X999" s="3"/>
-      <c r="Y999" s="3"/>
-      <c r="Z999" s="3"/>
-      <c r="AA999" s="3"/>
-      <c r="AB999" s="3"/>
-      <c r="AC999" s="3"/>
-      <c r="AD999" s="3"/>
-      <c r="AE999" s="3"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:AE1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -34316,8 +34330,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{00000000-000E-0000-0300-000001000000}">
-            <xm:f>COUNTIF(MatchScoutingData!$A$2:$A$999,CONCATENATE($A2,".",C$1)) = 1</xm:f>
+          <x14:cfRule type="expression" priority="5" id="{00000000-000E-0000-0300-000001000000}">
+            <xm:f>COUNTIF(MatchScoutingData!$A$2:$A$998,CONCATENATE($A2,".",C$1)) = 1</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="solid">
@@ -34327,8 +34341,8 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="4" id="{00000000-000E-0000-0300-000002000000}">
-            <xm:f>COUNTIF(MatchScoutingData!$A$2:$A$999,CONCATENATE($A2,".",C$1)) &gt; 1</xm:f>
+          <x14:cfRule type="expression" priority="6" id="{00000000-000E-0000-0300-000002000000}">
+            <xm:f>COUNTIF(MatchScoutingData!$A$2:$A$998,CONCATENATE($A2,".",C$1)) &gt; 1</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="solid">
@@ -34348,127 +34362,137 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AO3"/>
+  <dimension ref="A1:AS3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="AP1" sqref="AP1:AS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="41" width="5.5" customWidth="1"/>
+    <col min="2" max="45" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="42" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="34" t="s">
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="30" t="s">
-        <v>48</v>
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
+      <c r="AK1" s="41"/>
+      <c r="AL1" s="41"/>
+      <c r="AM1" s="42"/>
+      <c r="AN1" s="34" t="s">
+        <v>54</v>
       </c>
-      <c r="AO1" s="31"/>
-    </row>
-    <row r="2" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+    </row>
+    <row r="2" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="39" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="42" t="s">
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="42" t="s">
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="34" t="s">
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="48"/>
+      <c r="AF2" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="34" t="s">
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="38"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="33"/>
-    </row>
-    <row r="3" spans="1:41" ht="56" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AJ2" s="41"/>
+      <c r="AK2" s="41"/>
+      <c r="AL2" s="41"/>
+      <c r="AM2" s="42"/>
+      <c r="AN2" s="36"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+    </row>
+    <row r="3" spans="1:45" ht="56" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
@@ -34592,14 +34616,23 @@
       <c r="AO3" s="14" t="s">
         <v>49</v>
       </c>
+      <c r="AP3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AO3" xr:uid="{00000000-0009-0000-0000-000004000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AO34">
-      <sortCondition ref="A3:A34"/>
-    </sortState>
-  </autoFilter>
-  <mergeCells count="10">
+  <autoFilter ref="A3:AR3" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <mergeCells count="11">
+    <mergeCell ref="AP1:AS2"/>
     <mergeCell ref="AN1:AO2"/>
     <mergeCell ref="AF2:AH2"/>
     <mergeCell ref="AI2:AM2"/>
@@ -34617,7 +34650,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8299AA4A-5D09-AD47-9627-5C6D2535B1BB}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -34626,52 +34659,72 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="13" width="8" customWidth="1"/>
+    <col min="2" max="21" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="49" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-    </row>
-    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+    </row>
+    <row r="2" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="34" t="s">
+      <c r="E2" s="59"/>
+      <c r="F2" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="55" t="s">
+      <c r="G2" s="40"/>
+      <c r="H2" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="56"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="19"/>
       <c r="K2" s="20"/>
       <c r="L2" s="21"/>
       <c r="M2" s="22"/>
-    </row>
-    <row r="3" spans="1:13" ht="110" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+    </row>
+    <row r="3" spans="1:21" ht="110" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>6</v>
       </c>
@@ -34711,10 +34764,36 @@
       <c r="M3" s="27" t="s">
         <v>48</v>
       </c>
+      <c r="N3" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q3" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="S3" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="U3" s="31" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:M3" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
-  <mergeCells count="6">
+  <autoFilter ref="A3:U3" xr:uid="{8299AA4A-5D09-AD47-9627-5C6D2535B1BB}"/>
+  <mergeCells count="8">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="B2:C2"/>
@@ -34750,704 +34829,704 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="29" cm="1">
-        <f t="array" ref="A2">_xlfn._xlws.SORT(_xlfn.UNIQUE(MatchScoutingData!B2:B9998))</f>
+        <f t="array" ref="A2">_xlfn._xlws.SORT(_xlfn.UNIQUE(MatchScoutingData!B2:B9997))</f>
         <v>0</v>
       </c>
       <c r="B2" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A2)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="B3" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A3)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
       <c r="B4" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A4)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="29"/>
       <c r="B5" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A5)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="B6" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A6)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="29"/>
       <c r="B7" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A7)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
       <c r="B8" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A8)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="B9" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A9)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="B10" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A10)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="B11" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A11)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="29"/>
       <c r="B12" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A12)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="29"/>
       <c r="B13" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A13)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="B14" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A14)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="29"/>
       <c r="B15" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A15)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="29"/>
       <c r="B16" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A16)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="29"/>
       <c r="B17" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A17)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="29"/>
       <c r="B18" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A18)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="29"/>
       <c r="B19" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A19)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="29"/>
       <c r="B20" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A20)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="29"/>
       <c r="B21" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A21)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="29"/>
       <c r="B22" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A22)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="29"/>
       <c r="B23" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A23)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="29"/>
       <c r="B24" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A24)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="29"/>
       <c r="B25" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A25)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="29"/>
       <c r="B26" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A26)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="29"/>
       <c r="B27" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A27)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="29"/>
       <c r="B28" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A28)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="29"/>
       <c r="B29" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A29)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="29"/>
       <c r="B30" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A30)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="29"/>
       <c r="B31" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A31)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="29"/>
       <c r="B32" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A32)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="29"/>
       <c r="B33" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A33)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A33)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="29"/>
       <c r="B34" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A34)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A34)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="29"/>
       <c r="B35" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A35)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="29"/>
       <c r="B36" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A36)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A36)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="29"/>
       <c r="B37" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A37)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A37)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="29"/>
       <c r="B38" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A38)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A38)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="29"/>
       <c r="B39" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A39)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A39)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="29"/>
       <c r="B40" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A40)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A40)</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="29"/>
       <c r="B41" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A41)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A41)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="29"/>
       <c r="B42" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A42)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A42)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="29"/>
       <c r="B43" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A43)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A43)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
       <c r="B44" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A44)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A44)</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="29"/>
       <c r="B45" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A45)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A45)</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="29"/>
       <c r="B46" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A46)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A46)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="29"/>
       <c r="B47" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A47)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A47)</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="29"/>
       <c r="B48" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A48)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A48)</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="29"/>
       <c r="B49" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A49)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A49)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="29"/>
       <c r="B50" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A50)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A50)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="29"/>
       <c r="B51" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A51)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A51)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="29"/>
       <c r="B52" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A52)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A52)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="29"/>
       <c r="B53" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A53)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A53)</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="29"/>
       <c r="B54" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A54)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A54)</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="29"/>
       <c r="B55" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A55)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="29"/>
       <c r="B56" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A56)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A56)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="29"/>
       <c r="B57" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A57)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A57)</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="29"/>
       <c r="B58" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A58)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A58)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="29"/>
       <c r="B59" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A59)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A59)</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="29"/>
       <c r="B60" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A60)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A60)</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="29"/>
       <c r="B61" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A61)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A61)</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="29"/>
       <c r="B62" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A62)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A62)</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="29"/>
       <c r="B63" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A63)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A63)</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="29"/>
       <c r="B64" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A64)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A64)</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="29"/>
       <c r="B65" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A65)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A65)</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="29"/>
       <c r="B66" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A66)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A66)</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="29"/>
       <c r="B67" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A67)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A67)</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="29"/>
       <c r="B68" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A68)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A68)</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="29"/>
       <c r="B69" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A69)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A69)</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="29"/>
       <c r="B70" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A70)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A70)</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="29"/>
       <c r="B71" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A71)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A71)</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="29"/>
       <c r="B72" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A72)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A72)</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="29"/>
       <c r="B73" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A73)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A73)</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="29"/>
       <c r="B74" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A74)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A74)</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="29"/>
       <c r="B75" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A75)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A75)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="29"/>
       <c r="B76" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A76)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A76)</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="29"/>
       <c r="B77" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A77)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A77)</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="29"/>
       <c r="B78" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A78)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A78)</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="29"/>
       <c r="B79" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A79)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A79)</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="29"/>
       <c r="B80" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A80)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A80)</f>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="29"/>
       <c r="B81" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A81)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A81)</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="29"/>
       <c r="B82" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A82)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A82)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="29"/>
       <c r="B83" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A83)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A83)</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="29"/>
       <c r="B84" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A84)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A84)</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="29"/>
       <c r="B85" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A85)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A85)</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="29"/>
       <c r="B86" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A86)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A86)</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="29"/>
       <c r="B87" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A87)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A87)</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="29"/>
       <c r="B88" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A88)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A88)</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="29"/>
       <c r="B89" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A89)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A89)</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="29"/>
       <c r="B90" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A90)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A90)</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="29"/>
       <c r="B91" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A91)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A91)</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="29"/>
       <c r="B92" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A92)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A92)</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="29"/>
       <c r="B93" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A93)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A93)</f>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="29"/>
       <c r="B94" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A94)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A94)</f>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="29"/>
       <c r="B95" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A95)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A95)</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="29"/>
       <c r="B96" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A96)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A96)</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="29"/>
       <c r="B97" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A97)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A97)</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="29"/>
       <c r="B98" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A98)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A98)</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="29"/>
       <c r="B99" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A99)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A99)</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="29"/>
       <c r="B100" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A100)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A100)</f>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="29"/>
       <c r="B101" s="29">
-        <f>COUNTIF(MatchScoutingData!B$2:B$9998, $A101)</f>
+        <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A101)</f>
         <v>0</v>
       </c>
     </row>
@@ -35461,7 +35540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB4B0C7-8491-5245-AEE9-A2EE3051E88F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed some test data from Excel template.
</commit_message>
<xml_diff>
--- a/tba/tba_push_into_excel_template.xlsx
+++ b/tba/tba_push_into_excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnhurrell/Development/fairport-robotics/ScoutingPASSSync/tba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FA7D45-36AA-CC48-815D-41AE67A0F289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233E27AA-5ABC-2146-8860-097AD2A85909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
   <si>
     <t>Key</t>
   </si>
@@ -298,28 +298,7 @@
     <t>Post Barge Ranking</t>
   </si>
   <si>
-    <t>1.Red-1</t>
-  </si>
-  <si>
-    <t>Abyss Mortimer</t>
-  </si>
-  <si>
-    <t>2025nyrt</t>
-  </si>
-  <si>
     <t>Red-1</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>XXX</t>
   </si>
   <si>
     <t>Blue-1</t>
@@ -335,9 +314,6 @@
   </si>
   <si>
     <t>Red-3</t>
-  </si>
-  <si>
-    <t>2.Red-1</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1067,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1192,194 +1168,70 @@
       </c>
     </row>
     <row r="2" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="3">
-        <v>639</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3">
-        <v>2</v>
-      </c>
-      <c r="K2" s="3">
-        <v>3</v>
-      </c>
-      <c r="L2" s="3">
-        <v>4</v>
-      </c>
-      <c r="M2" s="3">
-        <v>5</v>
-      </c>
-      <c r="N2" s="3">
-        <v>6</v>
-      </c>
-      <c r="O2" s="3">
-        <v>7</v>
-      </c>
-      <c r="P2" s="3">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>9</v>
-      </c>
-      <c r="R2" s="3">
-        <v>10</v>
-      </c>
-      <c r="S2" s="3">
-        <v>11</v>
-      </c>
-      <c r="T2" s="3">
-        <v>12</v>
-      </c>
-      <c r="U2" s="3">
-        <v>13</v>
-      </c>
-      <c r="V2" s="3">
-        <v>14</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
     </row>
     <row r="3" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="3">
-        <v>639</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3">
-        <v>3</v>
-      </c>
-      <c r="L3" s="3">
-        <v>4</v>
-      </c>
-      <c r="M3" s="3">
-        <v>5</v>
-      </c>
-      <c r="N3" s="3">
-        <v>6</v>
-      </c>
-      <c r="O3" s="3">
-        <v>7</v>
-      </c>
-      <c r="P3" s="3">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>9</v>
-      </c>
-      <c r="R3" s="3">
-        <v>10</v>
-      </c>
-      <c r="S3" s="3">
-        <v>11</v>
-      </c>
-      <c r="T3" s="3">
-        <v>12</v>
-      </c>
-      <c r="U3" s="3">
-        <v>13</v>
-      </c>
-      <c r="V3" s="3">
-        <v>14</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
     </row>
     <row r="4" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -34455,22 +34307,22 @@
         <v>25</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -34979,19 +34831,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="str" cm="1">
-        <f t="array" ref="A2:A3">_xlfn._xlws.SORT(_xlfn.UNIQUE(MatchScoutingData!B2:B9997))</f>
-        <v>Abyss Mortimer</v>
+      <c r="A2" s="27" cm="1">
+        <f t="array" ref="A2">_xlfn._xlws.SORT(_xlfn.UNIQUE(MatchScoutingData!B2:B9997))</f>
+        <v>0</v>
       </c>
       <c r="B2" s="27">
         <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="27">
         <v>0</v>
       </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="27"/>
       <c r="B3" s="27">
         <f>COUNTIF(MatchScoutingData!B$2:B$9997, $A3)</f>
         <v>0</v>

</xml_diff>